<commit_message>
update handle with excel file
</commit_message>
<xml_diff>
--- a/profileid.xlsx
+++ b/profileid.xlsx
@@ -1,69 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dinhtiendat1901\WebstormProjects\gpm-auto\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81CD3C61-4088-44C1-8C3D-784FBF813EDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="28800" windowHeight="15345" xr2:uid="{719EEC14-E9E0-43BC-B950-5B8CF85C872C}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="28800" windowHeight="15345" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Trang_tính1" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="Trang_tính1" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="Sheet2" state="visible" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>cb490a1f-e98a-47f1-a33b-110f9731336b</t>
+    <t>28e0bc9e-21f8-4f4b-9f8e-753944213b65</t>
   </si>
   <si>
-    <t>526f015f-ba61-4ea7-b5b7-7a64bbe7819e</t>
-  </si>
-  <si>
-    <t>3376a2db-a62e-4768-aef0-f90efb4f14c1</t>
-  </si>
-  <si>
-    <t>8cf757d1-aa20-49d3-aa49-002e525a9b40</t>
-  </si>
-  <si>
-    <t>fafd1d6b-abfe-4d28-b279-ebabdef00a44</t>
+    <t>0183aab9-7022-4d38-a4b7-cc9a952e0601</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -86,12 +56,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -402,17 +371,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88BC27E5-C96A-4B34-9D0B-D493FFCB5A8F}">
-  <dimension ref="A1:A5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43.7109375" customWidth="1"/>
   </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -424,22 +407,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
</xml_diff>